<commit_message>
Add usage instructions in README
</commit_message>
<xml_diff>
--- a/spec/data/datafile.xlsx
+++ b/spec/data/datafile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Actores" sheetId="1" state="visible" r:id="rId2"/>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">Dominguez Servien </t>
   </si>
   <si>
-    <t xml:space="preserve">politico/empresario ganadero  </t>
+    <t xml:space="preserve">Empresario</t>
   </si>
   <si>
     <t xml:space="preserve">Juan Martin </t>
@@ -1419,11 +1419,11 @@
   </sheetPr>
   <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.01"/>
@@ -3242,7 +3242,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.57"/>
   </cols>
@@ -3745,14 +3745,14 @@
   </sheetPr>
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="83.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.71"/>
   </cols>
   <sheetData>
@@ -4708,7 +4708,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.86"/>

</xml_diff>